<commit_message>
Worked on Quality Scores on Dashboard
Related Work Items: #35, #46, #47, #62, #69
</commit_message>
<xml_diff>
--- a/HCL_HRIS/Files/Uploads/Audit Template.xlsx
+++ b/HCL_HRIS/Files/Uploads/Audit Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="20">
   <si>
     <t>Case ID</t>
   </si>
@@ -282,7 +282,49 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -569,7 +611,7 @@
   <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -628,13 +670,13 @@
         <v>16</v>
       </c>
       <c r="D2" s="4">
-        <v>51695613</v>
+        <v>51797296</v>
       </c>
       <c r="E2" s="4">
         <v>51787452</v>
       </c>
       <c r="F2" s="5">
-        <v>43810</v>
+        <v>43794</v>
       </c>
       <c r="G2" s="5">
         <v>43809</v>
@@ -662,14 +704,14 @@
       <c r="C3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="7">
-        <v>51695613</v>
+      <c r="D3" s="4">
+        <v>51797296</v>
       </c>
       <c r="E3" s="7">
         <v>51797122</v>
       </c>
       <c r="F3" s="8">
-        <v>43810</v>
+        <v>43804</v>
       </c>
       <c r="G3" s="8">
         <v>43809</v>
@@ -697,14 +739,14 @@
       <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="7">
-        <v>51695613</v>
+      <c r="D4" s="4">
+        <v>51797296</v>
       </c>
       <c r="E4" s="7">
         <v>51797122</v>
       </c>
       <c r="F4" s="8">
-        <v>43810</v>
+        <v>43803</v>
       </c>
       <c r="G4" s="8">
         <v>43809</v>
@@ -723,43 +765,109 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="11"/>
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4">
+        <v>51797296</v>
+      </c>
+      <c r="E5" s="4">
+        <v>51787452</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43805</v>
+      </c>
+      <c r="G5" s="5">
+        <v>43809</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="11"/>
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="4">
+        <v>51797296</v>
+      </c>
+      <c r="E6" s="4">
+        <v>51787452</v>
+      </c>
+      <c r="F6" s="5">
+        <v>43810</v>
+      </c>
+      <c r="G6" s="5">
+        <v>43809</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="11"/>
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4">
+        <v>51797296</v>
+      </c>
+      <c r="E7" s="4">
+        <v>51787452</v>
+      </c>
+      <c r="F7" s="5">
+        <v>43811</v>
+      </c>
+      <c r="G7" s="5">
+        <v>43809</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -770,9 +878,9 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="I8" s="9"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="11"/>
+      <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
@@ -1919,9 +2027,19 @@
       <c r="K96" s="13"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:K1048576">
+  <conditionalFormatting sqref="H1:K4 H9:K1048576">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",H1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:K6">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",H5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:K8">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",H1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Fail",H7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>